<commit_message>
README Update and debugging
</commit_message>
<xml_diff>
--- a/excel/optimized_portfolios_11-14-2021_github.xlsx
+++ b/excel/optimized_portfolios_11-14-2021_github.xlsx
@@ -1233,10 +1233,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>1.0362</v>
+        <v>1.036</v>
       </c>
       <c r="C4" s="5">
-        <v>3.516</v>
+        <v>3.5159</v>
       </c>
       <c r="D4" s="5">
         <v>3.8694</v>
@@ -1384,7 +1384,7 @@
         <v>0.3064</v>
       </c>
       <c r="I6" s="6">
-        <v>0.3578000000000001</v>
+        <v>0.3577</v>
       </c>
       <c r="J6" s="6">
         <v>0.4048</v>
@@ -1405,13 +1405,13 @@
         <v>0.6614</v>
       </c>
       <c r="P6" s="6">
-        <v>0.7135</v>
+        <v>0.7134</v>
       </c>
       <c r="Q6" s="6">
         <v>0.7657</v>
       </c>
       <c r="R6" s="6">
-        <v>0.8199000000000001</v>
+        <v>0.8198000000000001</v>
       </c>
       <c r="S6" s="6">
         <v>0.8726</v>
@@ -1959,22 +1959,22 @@
         <v>121</v>
       </c>
       <c r="B9" s="5">
-        <v>0.5426</v>
+        <v>0.5423</v>
       </c>
       <c r="C9" s="5">
-        <v>0.4957</v>
+        <v>0.4955</v>
       </c>
       <c r="D9" s="5">
-        <v>0.4207</v>
+        <v>0.4205</v>
       </c>
       <c r="E9" s="5">
-        <v>0.42</v>
+        <v>0.4198</v>
       </c>
       <c r="F9" s="5">
-        <v>0.5023</v>
+        <v>0.5021</v>
       </c>
       <c r="G9" s="5">
-        <v>0.4395</v>
+        <v>0.4394</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2120,19 +2120,19 @@
         <v>128</v>
       </c>
       <c r="B16" s="5">
-        <v>1.1327</v>
+        <v>1.1324</v>
       </c>
       <c r="C16" s="5">
-        <v>0.9664</v>
+        <v>0.9661999999999999</v>
       </c>
       <c r="D16" s="5">
-        <v>0.8421999999999999</v>
+        <v>0.8421</v>
       </c>
       <c r="E16" s="5">
-        <v>0.8106</v>
+        <v>0.8104</v>
       </c>
       <c r="F16" s="5">
-        <v>0.9213</v>
+        <v>0.9211</v>
       </c>
       <c r="G16" s="5">
         <v>0.826</v>
@@ -2166,22 +2166,22 @@
         <v>130</v>
       </c>
       <c r="B18" s="5">
-        <v>1.3215</v>
+        <v>1.3213</v>
       </c>
       <c r="C18" s="5">
-        <v>1.1048</v>
+        <v>1.1047</v>
       </c>
       <c r="D18" s="5">
-        <v>0.9608</v>
+        <v>0.9607</v>
       </c>
       <c r="E18" s="5">
-        <v>0.9167999999999999</v>
+        <v>0.9167</v>
       </c>
       <c r="F18" s="5">
         <v>1.0289</v>
       </c>
       <c r="G18" s="5">
-        <v>0.9409999999999999</v>
+        <v>0.9409</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -3188,7 +3188,7 @@
         <v>-0.0069</v>
       </c>
       <c r="C9" s="6">
-        <v>-0.0169</v>
+        <v>-0.017</v>
       </c>
       <c r="D9" s="6">
         <v>0.0896</v>
@@ -3197,7 +3197,7 @@
         <v>0.1351</v>
       </c>
       <c r="F9" s="6">
-        <v>0.1756</v>
+        <v>0.1757</v>
       </c>
       <c r="G9" s="6">
         <v>0.2202</v>
@@ -3807,10 +3807,10 @@
         <v>0.0536</v>
       </c>
       <c r="E9" s="6">
-        <v>0.08939999999999999</v>
+        <v>0.0893</v>
       </c>
       <c r="F9" s="6">
-        <v>0.1597</v>
+        <v>0.1598</v>
       </c>
       <c r="G9" s="6">
         <v>0.1311</v>
@@ -4106,10 +4106,10 @@
         <v>0</v>
       </c>
       <c r="E22" s="6">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F22" s="6">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="G22" s="6">
         <v>0</v>
@@ -4403,7 +4403,7 @@
         <v>0.7083</v>
       </c>
       <c r="G8" s="5">
-        <v>0.5547</v>
+        <v>0.5548</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4417,16 +4417,16 @@
         <v>0.046</v>
       </c>
       <c r="D9" s="5">
-        <v>0.1761</v>
+        <v>0.1762</v>
       </c>
       <c r="E9" s="5">
         <v>0.3447</v>
       </c>
       <c r="F9" s="5">
-        <v>0.6654</v>
+        <v>0.6656</v>
       </c>
       <c r="G9" s="5">
-        <v>0.5241</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4624,10 +4624,10 @@
         <v>0.0451</v>
       </c>
       <c r="D18" s="5">
-        <v>0.1168</v>
+        <v>0.1169</v>
       </c>
       <c r="E18" s="5">
-        <v>0.2753</v>
+        <v>0.2754</v>
       </c>
       <c r="F18" s="5">
         <v>0.5217000000000001</v>
@@ -4895,10 +4895,10 @@
         <v>2.5053</v>
       </c>
       <c r="E3" s="5">
-        <v>4.1015</v>
+        <v>4.1016</v>
       </c>
       <c r="F3" s="5">
-        <v>3.6421</v>
+        <v>3.642</v>
       </c>
       <c r="G3" s="5">
         <v>2.5851</v>
@@ -4921,7 +4921,7 @@
         <v>6.6238</v>
       </c>
       <c r="F4" s="5">
-        <v>5.6001</v>
+        <v>5.6</v>
       </c>
       <c r="G4" s="5">
         <v>2.6344</v>
@@ -4964,10 +4964,10 @@
         <v>5.2421</v>
       </c>
       <c r="E6" s="5">
-        <v>6.6602</v>
+        <v>6.6601</v>
       </c>
       <c r="F6" s="5">
-        <v>6.612</v>
+        <v>6.6119</v>
       </c>
       <c r="G6" s="5">
         <v>2.5251</v>
@@ -4987,10 +4987,10 @@
         <v>4.8161</v>
       </c>
       <c r="E7" s="5">
-        <v>6.8489</v>
+        <v>6.8488</v>
       </c>
       <c r="F7" s="5">
-        <v>6.5886</v>
+        <v>6.5885</v>
       </c>
       <c r="G7" s="5">
         <v>2.418</v>
@@ -5024,22 +5024,22 @@
         <v>121</v>
       </c>
       <c r="B9" s="5">
-        <v>-11.5552</v>
+        <v>-11.5696</v>
       </c>
       <c r="C9" s="5">
-        <v>2.2325</v>
+        <v>2.2327</v>
       </c>
       <c r="D9" s="5">
-        <v>3.9895</v>
+        <v>3.9908</v>
       </c>
       <c r="E9" s="5">
-        <v>6.5365</v>
+        <v>6.5362</v>
       </c>
       <c r="F9" s="5">
-        <v>6.1878</v>
+        <v>6.1889</v>
       </c>
       <c r="G9" s="5">
-        <v>2.2881</v>
+        <v>2.2877</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5047,19 +5047,19 @@
         <v>122</v>
       </c>
       <c r="B10" s="5">
-        <v>-9.029400000000001</v>
+        <v>-9.028600000000001</v>
       </c>
       <c r="C10" s="5">
-        <v>2.2338</v>
+        <v>2.2339</v>
       </c>
       <c r="D10" s="5">
         <v>3.7061</v>
       </c>
       <c r="E10" s="5">
-        <v>6.2857</v>
+        <v>6.2858</v>
       </c>
       <c r="F10" s="5">
-        <v>5.9865</v>
+        <v>5.9867</v>
       </c>
       <c r="G10" s="5">
         <v>2.2331</v>
@@ -5185,10 +5185,10 @@
         <v>128</v>
       </c>
       <c r="B16" s="5">
-        <v>-2.2932</v>
+        <v>-2.295</v>
       </c>
       <c r="C16" s="5">
-        <v>2.5801</v>
+        <v>2.58</v>
       </c>
       <c r="D16" s="5">
         <v>2.7667</v>
@@ -5200,7 +5200,7 @@
         <v>5.2648</v>
       </c>
       <c r="G16" s="5">
-        <v>1.9431</v>
+        <v>1.9432</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -5214,7 +5214,7 @@
         <v>2.6235</v>
       </c>
       <c r="D17" s="5">
-        <v>2.6883</v>
+        <v>2.6882</v>
       </c>
       <c r="E17" s="5">
         <v>5.1137</v>
@@ -5231,22 +5231,22 @@
         <v>130</v>
       </c>
       <c r="B18" s="5">
-        <v>-2.0371</v>
+        <v>-2.0375</v>
       </c>
       <c r="C18" s="5">
-        <v>2.5096</v>
+        <v>2.5095</v>
       </c>
       <c r="D18" s="5">
-        <v>2.5516</v>
+        <v>2.5517</v>
       </c>
       <c r="E18" s="5">
-        <v>5.0415</v>
+        <v>5.0416</v>
       </c>
       <c r="F18" s="5">
-        <v>5.198</v>
+        <v>5.1979</v>
       </c>
       <c r="G18" s="5">
-        <v>1.8447</v>
+        <v>1.8448</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -5511,7 +5511,7 @@
         <v>0.4565</v>
       </c>
       <c r="G3" s="5">
-        <v>0.951</v>
+        <v>0.9507</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5534,7 +5534,7 @@
         <v>0.9562</v>
       </c>
       <c r="G4" s="5">
-        <v>1.1145</v>
+        <v>1.1144</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5557,7 +5557,7 @@
         <v>1.034</v>
       </c>
       <c r="G5" s="5">
-        <v>1.1408</v>
+        <v>1.1407</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5580,7 +5580,7 @@
         <v>1.0868</v>
       </c>
       <c r="G6" s="5">
-        <v>1.1447</v>
+        <v>1.1448</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5643,13 +5643,13 @@
         <v>1.552</v>
       </c>
       <c r="E9" s="5">
-        <v>1.347</v>
+        <v>1.3458</v>
       </c>
       <c r="F9" s="5">
-        <v>1.1333</v>
+        <v>1.1345</v>
       </c>
       <c r="G9" s="5">
-        <v>1.1327</v>
+        <v>1.133</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5672,7 +5672,7 @@
         <v>1.153</v>
       </c>
       <c r="G10" s="5">
-        <v>1.1292</v>
+        <v>1.1291</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -5695,7 +5695,7 @@
         <v>1.1357</v>
       </c>
       <c r="G11" s="5">
-        <v>1.1167</v>
+        <v>1.1166</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -5807,10 +5807,10 @@
         <v>1.3141</v>
       </c>
       <c r="F16" s="5">
-        <v>1.0887</v>
+        <v>1.0889</v>
       </c>
       <c r="G16" s="5">
-        <v>1.0855</v>
+        <v>1.0857</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -5856,7 +5856,7 @@
         <v>1.0746</v>
       </c>
       <c r="G18" s="5">
-        <v>1.0723</v>
+        <v>1.0722</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -5876,7 +5876,7 @@
         <v>1.2835</v>
       </c>
       <c r="F19" s="5">
-        <v>1.0665</v>
+        <v>1.0667</v>
       </c>
       <c r="G19" s="5">
         <v>1.0644</v>
@@ -5902,7 +5902,7 @@
         <v>1.0544</v>
       </c>
       <c r="G20" s="5">
-        <v>1.0572</v>
+        <v>1.0573</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -5925,7 +5925,7 @@
         <v>1.0712</v>
       </c>
       <c r="G21" s="5">
-        <v>1.0496</v>
+        <v>1.0497</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -6118,7 +6118,7 @@
         <v>1.014</v>
       </c>
       <c r="E3" s="5">
-        <v>1.675</v>
+        <v>1.6751</v>
       </c>
       <c r="F3" s="5">
         <v>0.8337</v>
@@ -6250,19 +6250,19 @@
         <v>-0.9824000000000001</v>
       </c>
       <c r="C9" s="5">
-        <v>-0.09710000000000001</v>
+        <v>-0.0969</v>
       </c>
       <c r="D9" s="5">
         <v>2.8877</v>
       </c>
       <c r="E9" s="5">
-        <v>3.6119</v>
+        <v>3.6108</v>
       </c>
       <c r="F9" s="5">
-        <v>3.1911</v>
+        <v>3.1927</v>
       </c>
       <c r="G9" s="5">
-        <v>2.1484</v>
+        <v>2.1481</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6270,7 +6270,7 @@
         <v>122</v>
       </c>
       <c r="B10" s="5">
-        <v>-0.9137999999999999</v>
+        <v>-0.9137</v>
       </c>
       <c r="C10" s="5">
         <v>-0.0944</v>
@@ -6279,10 +6279,10 @@
         <v>2.9574</v>
       </c>
       <c r="E10" s="5">
-        <v>3.7397</v>
+        <v>3.7398</v>
       </c>
       <c r="F10" s="5">
-        <v>3.1546</v>
+        <v>3.1547</v>
       </c>
       <c r="G10" s="5">
         <v>2.1802</v>
@@ -6299,7 +6299,7 @@
         <v>-0.2135</v>
       </c>
       <c r="D11" s="5">
-        <v>2.9989</v>
+        <v>2.999</v>
       </c>
       <c r="E11" s="5">
         <v>3.7344</v>
@@ -6408,22 +6408,22 @@
         <v>128</v>
       </c>
       <c r="B16" s="5">
-        <v>-0.6025</v>
+        <v>-0.6026</v>
       </c>
       <c r="C16" s="5">
         <v>-0.07439999999999999</v>
       </c>
       <c r="D16" s="5">
-        <v>2.9696</v>
+        <v>2.9692</v>
       </c>
       <c r="E16" s="5">
-        <v>4.0947</v>
+        <v>4.0943</v>
       </c>
       <c r="F16" s="5">
-        <v>2.9502</v>
+        <v>2.95</v>
       </c>
       <c r="G16" s="5">
-        <v>2.1835</v>
+        <v>2.1836</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -6454,22 +6454,22 @@
         <v>130</v>
       </c>
       <c r="B18" s="5">
-        <v>-0.6939</v>
+        <v>-0.694</v>
       </c>
       <c r="C18" s="5">
-        <v>-0.2346</v>
+        <v>-0.2344</v>
       </c>
       <c r="D18" s="5">
-        <v>2.8608</v>
+        <v>2.8611</v>
       </c>
       <c r="E18" s="5">
-        <v>4.2267</v>
+        <v>4.2268</v>
       </c>
       <c r="F18" s="5">
         <v>2.9736</v>
       </c>
       <c r="G18" s="5">
-        <v>2.0993</v>
+        <v>2.0994</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -6532,7 +6532,7 @@
         <v>2.5405</v>
       </c>
       <c r="E21" s="5">
-        <v>3.9351</v>
+        <v>3.935</v>
       </c>
       <c r="F21" s="5">
         <v>3.0971</v>
@@ -6714,7 +6714,7 @@
         <v>-0.1697</v>
       </c>
       <c r="G2" s="5">
-        <v>0.6266</v>
+        <v>0.6264999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6863,19 +6863,19 @@
         <v>-0.5319</v>
       </c>
       <c r="C9" s="5">
-        <v>1.4312</v>
+        <v>1.4311</v>
       </c>
       <c r="D9" s="5">
-        <v>1.9946</v>
+        <v>1.9953</v>
       </c>
       <c r="E9" s="5">
-        <v>2.846</v>
+        <v>2.8454</v>
       </c>
       <c r="F9" s="5">
-        <v>1.9017</v>
+        <v>1.9024</v>
       </c>
       <c r="G9" s="5">
-        <v>0.8075</v>
+        <v>0.8073</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6886,7 +6886,7 @@
         <v>-0.5089</v>
       </c>
       <c r="C10" s="5">
-        <v>1.5216</v>
+        <v>1.5217</v>
       </c>
       <c r="D10" s="5">
         <v>1.8534</v>
@@ -6895,7 +6895,7 @@
         <v>2.7633</v>
       </c>
       <c r="F10" s="5">
-        <v>1.7891</v>
+        <v>1.7892</v>
       </c>
       <c r="G10" s="5">
         <v>0.7877</v>
@@ -7021,22 +7021,22 @@
         <v>128</v>
       </c>
       <c r="B16" s="5">
-        <v>-0.3986</v>
+        <v>-0.3987</v>
       </c>
       <c r="C16" s="5">
-        <v>1.8852</v>
+        <v>1.885</v>
       </c>
       <c r="D16" s="5">
-        <v>1.238</v>
+        <v>1.2381</v>
       </c>
       <c r="E16" s="5">
-        <v>2.2033</v>
+        <v>2.2034</v>
       </c>
       <c r="F16" s="5">
-        <v>1.4477</v>
+        <v>1.4478</v>
       </c>
       <c r="G16" s="5">
-        <v>0.6816</v>
+        <v>0.6817</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -7067,16 +7067,16 @@
         <v>130</v>
       </c>
       <c r="B18" s="5">
-        <v>-0.4036</v>
+        <v>-0.4037</v>
       </c>
       <c r="C18" s="5">
-        <v>1.7893</v>
+        <v>1.7894</v>
       </c>
       <c r="D18" s="5">
-        <v>1.1349</v>
+        <v>1.135</v>
       </c>
       <c r="E18" s="5">
-        <v>2.1393</v>
+        <v>2.1394</v>
       </c>
       <c r="F18" s="5">
         <v>1.4099</v>
@@ -7473,19 +7473,19 @@
         <v>121</v>
       </c>
       <c r="B9" s="5">
-        <v>-0.222</v>
+        <v>-0.2219</v>
       </c>
       <c r="C9" s="5">
         <v>-0.3849</v>
       </c>
       <c r="D9" s="5">
-        <v>0.0774</v>
+        <v>0.07729999999999999</v>
       </c>
       <c r="E9" s="5">
-        <v>0.0176</v>
+        <v>0.0174</v>
       </c>
       <c r="F9" s="5">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G9" s="5">
         <v>-0.0067</v>
@@ -7637,16 +7637,16 @@
         <v>-0.3245</v>
       </c>
       <c r="C16" s="5">
-        <v>-0.0419</v>
+        <v>-0.0421</v>
       </c>
       <c r="D16" s="5">
-        <v>0.2851</v>
+        <v>0.285</v>
       </c>
       <c r="E16" s="5">
-        <v>0.2219</v>
+        <v>0.2218</v>
       </c>
       <c r="F16" s="5">
-        <v>0.1147</v>
+        <v>0.1146</v>
       </c>
       <c r="G16" s="5">
         <v>0.06510000000000001</v>
@@ -7680,10 +7680,10 @@
         <v>130</v>
       </c>
       <c r="B18" s="5">
-        <v>-0.3628</v>
+        <v>-0.3629</v>
       </c>
       <c r="C18" s="5">
-        <v>0.0294</v>
+        <v>0.0293</v>
       </c>
       <c r="D18" s="5">
         <v>0.3262</v>
@@ -8050,7 +8050,7 @@
         <v>0.0369</v>
       </c>
       <c r="T2" s="6">
-        <v>0.0455</v>
+        <v>0.0454</v>
       </c>
       <c r="U2" s="6">
         <v>0.0291</v>
@@ -8397,10 +8397,10 @@
         <v>0.1542</v>
       </c>
       <c r="S6" s="6">
-        <v>0.0907</v>
+        <v>0.09080000000000001</v>
       </c>
       <c r="T6" s="6">
-        <v>0.0319</v>
+        <v>0.032</v>
       </c>
       <c r="U6" s="6">
         <v>0</v>
@@ -9085,7 +9085,7 @@
         <v>0.0922</v>
       </c>
       <c r="S14" s="6">
-        <v>0.07820000000000001</v>
+        <v>0.0781</v>
       </c>
       <c r="T14" s="6">
         <v>0.06510000000000001</v>
@@ -9281,13 +9281,13 @@
         <v>0.0927</v>
       </c>
       <c r="Z16" s="6">
-        <v>0.1102</v>
+        <v>0.1101</v>
       </c>
       <c r="AA16" s="6">
         <v>0.1278</v>
       </c>
       <c r="AB16" s="6">
-        <v>0.0888</v>
+        <v>0.0887</v>
       </c>
       <c r="AC16" s="6">
         <v>0.1226</v>
@@ -10043,7 +10043,7 @@
         <v>0.1064</v>
       </c>
       <c r="S25" s="6">
-        <v>0.134</v>
+        <v>0.1339</v>
       </c>
       <c r="T25" s="6">
         <v>0.1551</v>
@@ -10834,16 +10834,16 @@
         <v>-0.0105</v>
       </c>
       <c r="C9" s="6">
-        <v>0.0311</v>
+        <v>0.031</v>
       </c>
       <c r="D9" s="6">
         <v>0.1384</v>
       </c>
       <c r="E9" s="6">
-        <v>0.267</v>
+        <v>0.2669</v>
       </c>
       <c r="F9" s="6">
-        <v>0.5041</v>
+        <v>0.5043</v>
       </c>
       <c r="G9" s="6">
         <v>0.4459</v>
@@ -11044,10 +11044,10 @@
         <v>0.0378</v>
       </c>
       <c r="D18" s="6">
-        <v>0.1075</v>
+        <v>0.1076</v>
       </c>
       <c r="E18" s="6">
-        <v>0.2491</v>
+        <v>0.2492</v>
       </c>
       <c r="F18" s="6">
         <v>0.4624</v>
@@ -11344,7 +11344,7 @@
         <v>0.0786</v>
       </c>
       <c r="G4" s="6">
-        <v>0.0355</v>
+        <v>0.0354</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -11456,10 +11456,10 @@
         <v>0.0554</v>
       </c>
       <c r="F9" s="6">
-        <v>0.1745</v>
+        <v>0.1744</v>
       </c>
       <c r="G9" s="6">
-        <v>0.0992</v>
+        <v>0.09909999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -11614,7 +11614,7 @@
         <v>0.0411</v>
       </c>
       <c r="E16" s="6">
-        <v>0.1069</v>
+        <v>0.1068</v>
       </c>
       <c r="F16" s="6">
         <v>0.3041</v>
@@ -12217,7 +12217,7 @@
         <v>0.0448</v>
       </c>
       <c r="Z4" s="6">
-        <v>0.0427</v>
+        <v>0.0428</v>
       </c>
       <c r="AA4" s="6">
         <v>0.0402</v>
@@ -13252,13 +13252,13 @@
         <v>0.116</v>
       </c>
       <c r="Z16" s="6">
-        <v>0.1302</v>
+        <v>0.1301</v>
       </c>
       <c r="AA16" s="6">
         <v>0.1428</v>
       </c>
       <c r="AB16" s="6">
-        <v>0.0941</v>
+        <v>0.094</v>
       </c>
       <c r="AC16" s="6">
         <v>0.1236</v>
@@ -13394,7 +13394,7 @@
         <v>0.0272</v>
       </c>
       <c r="P18" s="6">
-        <v>0.008200000000000001</v>
+        <v>0.0083</v>
       </c>
       <c r="Q18" s="6">
         <v>0</v>
@@ -14014,7 +14014,7 @@
         <v>0.2311</v>
       </c>
       <c r="S25" s="6">
-        <v>0.2719</v>
+        <v>0.2718</v>
       </c>
       <c r="T25" s="6">
         <v>0.2939</v>
@@ -14388,7 +14388,7 @@
         <v>0.1931</v>
       </c>
       <c r="AB29" s="6">
-        <v>0.1831</v>
+        <v>0.1832</v>
       </c>
       <c r="AC29" s="6">
         <v>0.1742</v>
@@ -14965,7 +14965,7 @@
         <v>0.9500000000000002</v>
       </c>
       <c r="I6" s="6">
-        <v>0.9476000000000002</v>
+        <v>0.9475000000000002</v>
       </c>
       <c r="J6" s="6">
         <v>0.9443000000000001</v>
@@ -14986,13 +14986,13 @@
         <v>0.9476000000000001</v>
       </c>
       <c r="P6" s="6">
-        <v>0.9476000000000002</v>
+        <v>0.9475000000000002</v>
       </c>
       <c r="Q6" s="6">
         <v>0.9475</v>
       </c>
       <c r="R6" s="6">
-        <v>0.9845000000000002</v>
+        <v>0.9844000000000002</v>
       </c>
       <c r="S6" s="6">
         <v>0.9976</v>
@@ -15051,13 +15051,13 @@
         <v>0.7976</v>
       </c>
       <c r="P7" s="6">
-        <v>0.7976000000000001</v>
+        <v>0.7975000000000001</v>
       </c>
       <c r="Q7" s="6">
         <v>0.7975</v>
       </c>
       <c r="R7" s="6">
-        <v>0.7975000000000001</v>
+        <v>0.7974000000000001</v>
       </c>
       <c r="S7" s="6">
         <v>0.7976000000000001</v>
@@ -15095,7 +15095,7 @@
         <v>0.3</v>
       </c>
       <c r="I8" s="6">
-        <v>0.2976</v>
+        <v>0.2975</v>
       </c>
       <c r="J8" s="6">
         <v>0.2943</v>
@@ -15225,7 +15225,7 @@
         <v>0.2464</v>
       </c>
       <c r="I10" s="6">
-        <v>0.2978</v>
+        <v>0.2977</v>
       </c>
       <c r="J10" s="6">
         <v>0.3448000000000001</v>
@@ -15246,13 +15246,13 @@
         <v>0.5914</v>
       </c>
       <c r="P10" s="6">
-        <v>0.6435000000000001</v>
+        <v>0.6434000000000001</v>
       </c>
       <c r="Q10" s="6">
         <v>0.6957000000000001</v>
       </c>
       <c r="R10" s="6">
-        <v>0.7499000000000001</v>
+        <v>0.7498000000000001</v>
       </c>
       <c r="S10" s="6">
         <v>0.8026</v>
@@ -15485,7 +15485,7 @@
         <v>0.2564</v>
       </c>
       <c r="I14" s="6">
-        <v>0.3078</v>
+        <v>0.3077</v>
       </c>
       <c r="J14" s="6">
         <v>0.3548000000000001</v>
@@ -15506,13 +15506,13 @@
         <v>0.6014</v>
       </c>
       <c r="P14" s="6">
-        <v>0.6535000000000001</v>
+        <v>0.6534000000000001</v>
       </c>
       <c r="Q14" s="6">
         <v>0.7057</v>
       </c>
       <c r="R14" s="6">
-        <v>0.7599000000000001</v>
+        <v>0.7598000000000001</v>
       </c>
       <c r="S14" s="6">
         <v>0.8126</v>
@@ -15940,7 +15940,7 @@
         <v>0.1064</v>
       </c>
       <c r="I21" s="6">
-        <v>0.134</v>
+        <v>0.1339</v>
       </c>
       <c r="J21" s="6">
         <v>0.1551</v>
@@ -15961,13 +15961,13 @@
         <v>0.3122</v>
       </c>
       <c r="P21" s="6">
-        <v>0.3635</v>
+        <v>0.3634000000000001</v>
       </c>
       <c r="Q21" s="6">
         <v>0.4157</v>
       </c>
       <c r="R21" s="6">
-        <v>0.4699</v>
+        <v>0.4698</v>
       </c>
       <c r="S21" s="6">
         <v>0.5226</v>
@@ -16200,7 +16200,7 @@
         <v>0.7604</v>
       </c>
       <c r="I25" s="6">
-        <v>0.758</v>
+        <v>0.7579</v>
       </c>
       <c r="J25" s="6">
         <v>0.7579</v>
@@ -16221,13 +16221,13 @@
         <v>0.7579999999999999</v>
       </c>
       <c r="P25" s="6">
-        <v>0.758</v>
+        <v>0.7579</v>
       </c>
       <c r="Q25" s="6">
         <v>0.7579</v>
       </c>
       <c r="R25" s="6">
-        <v>0.7579</v>
+        <v>0.7578</v>
       </c>
       <c r="S25" s="6">
         <v>0.758</v>
@@ -16265,7 +16265,7 @@
         <v>0.3064</v>
       </c>
       <c r="I26" s="6">
-        <v>0.3578000000000001</v>
+        <v>0.3577</v>
       </c>
       <c r="J26" s="6">
         <v>0.4048</v>
@@ -16286,13 +16286,13 @@
         <v>0.6614</v>
       </c>
       <c r="P26" s="6">
-        <v>0.7135</v>
+        <v>0.7134</v>
       </c>
       <c r="Q26" s="6">
         <v>0.7657</v>
       </c>
       <c r="R26" s="6">
-        <v>0.8199000000000001</v>
+        <v>0.8198000000000001</v>
       </c>
       <c r="S26" s="6">
         <v>0.8726</v>
@@ -16395,7 +16395,7 @@
         <v>0.3</v>
       </c>
       <c r="I28" s="6">
-        <v>0.2976</v>
+        <v>0.2975</v>
       </c>
       <c r="J28" s="6">
         <v>0.2975</v>
@@ -16877,7 +16877,7 @@
         <v>0.9833999999999999</v>
       </c>
       <c r="F6" s="6">
-        <v>0.9699</v>
+        <v>0.97</v>
       </c>
       <c r="G6" s="6">
         <v>0.9763000000000002</v>
@@ -16886,7 +16886,7 @@
         <v>0.9810999999999999</v>
       </c>
       <c r="I6" s="6">
-        <v>0.9845000000000002</v>
+        <v>0.9844000000000002</v>
       </c>
       <c r="J6" s="6">
         <v>0.9867999999999999</v>
@@ -16907,7 +16907,7 @@
         <v>0.9932000000000001</v>
       </c>
       <c r="P6" s="6">
-        <v>0.994</v>
+        <v>0.9939999999999999</v>
       </c>
       <c r="Q6" s="6">
         <v>0.9947000000000001</v>
@@ -16942,7 +16942,7 @@
         <v>0.2327</v>
       </c>
       <c r="F7" s="6">
-        <v>0.23</v>
+        <v>0.2301</v>
       </c>
       <c r="G7" s="6">
         <v>0.2809</v>
@@ -16951,7 +16951,7 @@
         <v>0.3700000000000001</v>
       </c>
       <c r="I7" s="6">
-        <v>0.4395999999999999</v>
+        <v>0.4394999999999999</v>
       </c>
       <c r="J7" s="6">
         <v>0.5005000000000001</v>
@@ -16972,7 +16972,7 @@
         <v>0.6759999999999999</v>
       </c>
       <c r="P7" s="6">
-        <v>0.6984</v>
+        <v>0.6983</v>
       </c>
       <c r="Q7" s="6">
         <v>0.7182999999999999</v>
@@ -17037,7 +17037,7 @@
         <v>0.3238</v>
       </c>
       <c r="P8" s="6">
-        <v>0.3015</v>
+        <v>0.3016</v>
       </c>
       <c r="Q8" s="6">
         <v>0.2818</v>
@@ -17146,7 +17146,7 @@
         <v>0.5787</v>
       </c>
       <c r="I10" s="6">
-        <v>0.6375999999999999</v>
+        <v>0.6375</v>
       </c>
       <c r="J10" s="6">
         <v>0.6823</v>
@@ -17406,7 +17406,7 @@
         <v>0.6162</v>
       </c>
       <c r="I14" s="6">
-        <v>0.6711</v>
+        <v>0.671</v>
       </c>
       <c r="J14" s="6">
         <v>0.7126</v>
@@ -17687,7 +17687,7 @@
         <v>0.0448</v>
       </c>
       <c r="P18" s="6">
-        <v>0.0427</v>
+        <v>0.0428</v>
       </c>
       <c r="Q18" s="6">
         <v>0.0402</v>
@@ -17861,7 +17861,7 @@
         <v>0.2311</v>
       </c>
       <c r="I21" s="6">
-        <v>0.2719</v>
+        <v>0.2718</v>
       </c>
       <c r="J21" s="6">
         <v>0.2939</v>
@@ -17882,13 +17882,13 @@
         <v>0.4069</v>
       </c>
       <c r="P21" s="6">
-        <v>0.4448</v>
+        <v>0.4447</v>
       </c>
       <c r="Q21" s="6">
         <v>0.4792</v>
       </c>
       <c r="R21" s="6">
-        <v>0.5131</v>
+        <v>0.513</v>
       </c>
       <c r="S21" s="6">
         <v>0.5413</v>
@@ -18018,7 +18018,7 @@
         <v>0.2503</v>
       </c>
       <c r="R23" s="6">
-        <v>0.237</v>
+        <v>0.2371</v>
       </c>
       <c r="S23" s="6">
         <v>0.2251</v>
@@ -18077,7 +18077,7 @@
         <v>0.3238</v>
       </c>
       <c r="P24" s="6">
-        <v>0.3015</v>
+        <v>0.3016</v>
       </c>
       <c r="Q24" s="6">
         <v>0.2818</v>
@@ -18112,7 +18112,7 @@
         <v>0.1686</v>
       </c>
       <c r="F25" s="6">
-        <v>0.1331</v>
+        <v>0.1332</v>
       </c>
       <c r="G25" s="6">
         <v>0.196</v>
@@ -18121,7 +18121,7 @@
         <v>0.2936</v>
       </c>
       <c r="I25" s="6">
-        <v>0.3703</v>
+        <v>0.3702</v>
       </c>
       <c r="J25" s="6">
         <v>0.4373</v>
@@ -18142,7 +18142,7 @@
         <v>0.6322</v>
       </c>
       <c r="P25" s="6">
-        <v>0.6573</v>
+        <v>0.6572</v>
       </c>
       <c r="Q25" s="6">
         <v>0.6795</v>
@@ -18186,7 +18186,7 @@
         <v>0.8575999999999999</v>
       </c>
       <c r="I26" s="6">
-        <v>0.8818</v>
+        <v>0.8817</v>
       </c>
       <c r="J26" s="6">
         <v>0.8993999999999999</v>
@@ -18242,7 +18242,7 @@
         <v>0.1521</v>
       </c>
       <c r="F27" s="6">
-        <v>0.1031</v>
+        <v>0.1032</v>
       </c>
       <c r="G27" s="6">
         <v>0.0683</v>
@@ -18372,7 +18372,7 @@
         <v>0.1462</v>
       </c>
       <c r="F29" s="6">
-        <v>0.1024</v>
+        <v>0.1025</v>
       </c>
       <c r="G29" s="6">
         <v>0.0683</v>
@@ -18841,7 +18841,7 @@
         <v>0.0741</v>
       </c>
       <c r="E9" s="6">
-        <v>0.1448</v>
+        <v>0.1447</v>
       </c>
       <c r="F9" s="6">
         <v>0.3342</v>
@@ -18999,7 +18999,7 @@
         <v>0.0454</v>
       </c>
       <c r="D16" s="6">
-        <v>0.1059</v>
+        <v>0.1058</v>
       </c>
       <c r="E16" s="6">
         <v>0.2268</v>
@@ -19445,22 +19445,22 @@
         <v>121</v>
       </c>
       <c r="B9" s="5">
-        <v>-0.7955</v>
+        <v>-0.7956</v>
       </c>
       <c r="C9" s="5">
-        <v>1.6148</v>
+        <v>1.6145</v>
       </c>
       <c r="D9" s="5">
-        <v>2.4701</v>
+        <v>2.4704</v>
       </c>
       <c r="E9" s="5">
-        <v>3.6983</v>
+        <v>3.6978</v>
       </c>
       <c r="F9" s="5">
-        <v>3.9946</v>
+        <v>3.9957</v>
       </c>
       <c r="G9" s="5">
-        <v>1.9824</v>
+        <v>1.9822</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -19468,7 +19468,7 @@
         <v>122</v>
       </c>
       <c r="B10" s="5">
-        <v>-0.7358</v>
+        <v>-0.7357</v>
       </c>
       <c r="C10" s="5">
         <v>1.7216</v>
@@ -19477,13 +19477,13 @@
         <v>2.407</v>
       </c>
       <c r="E10" s="5">
-        <v>3.6803</v>
+        <v>3.6804</v>
       </c>
       <c r="F10" s="5">
         <v>3.9347</v>
       </c>
       <c r="G10" s="5">
-        <v>1.9417</v>
+        <v>1.9416</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -19606,10 +19606,10 @@
         <v>128</v>
       </c>
       <c r="B16" s="5">
-        <v>-0.49</v>
+        <v>-0.4901</v>
       </c>
       <c r="C16" s="5">
-        <v>2.0193</v>
+        <v>2.0191</v>
       </c>
       <c r="D16" s="5">
         <v>2.0362</v>
@@ -19655,13 +19655,13 @@
         <v>-0.5006</v>
       </c>
       <c r="C18" s="5">
-        <v>1.9636</v>
+        <v>1.9637</v>
       </c>
       <c r="D18" s="5">
-        <v>1.9196</v>
+        <v>1.9197</v>
       </c>
       <c r="E18" s="5">
-        <v>3.4523</v>
+        <v>3.4524</v>
       </c>
       <c r="F18" s="5">
         <v>3.6562</v>
@@ -19756,7 +19756,7 @@
         <v>1.8268</v>
       </c>
       <c r="F22" s="5">
-        <v>2.556</v>
+        <v>2.5561</v>
       </c>
       <c r="G22" s="5">
         <v>1.0032</v>
@@ -20268,7 +20268,7 @@
         <v>0.0186</v>
       </c>
       <c r="C18" s="6">
-        <v>0.0254</v>
+        <v>0.0253</v>
       </c>
       <c r="D18" s="6">
         <v>0.0585</v>
@@ -20280,7 +20280,7 @@
         <v>0.1418</v>
       </c>
       <c r="G18" s="6">
-        <v>0.2235</v>
+        <v>0.2234</v>
       </c>
     </row>
     <row r="19" spans="1:7">

</xml_diff>